<commit_message>
Recent Additions, In need of touch ups
</commit_message>
<xml_diff>
--- a/data/Nordic_dry.xlsx
+++ b/data/Nordic_dry.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFEB96B-9FCA-4EA1-B064-1CD21A6BD745}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7500D6-C2EF-495F-B4F8-1BB3C93E0A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-21600" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Node Parameters" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,20 @@
     <sheet name="DC Link Parameters" sheetId="3" r:id="rId3"/>
     <sheet name="Declarations" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -236,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -250,35 +263,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -305,9 +306,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -345,9 +346,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -380,26 +381,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -432,26 +416,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -627,26 +594,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -666,7 +633,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -686,7 +653,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -706,7 +673,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -726,7 +693,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -746,7 +713,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -766,7 +733,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -786,7 +753,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -806,7 +773,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -826,7 +793,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -846,7 +813,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -866,7 +833,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -877,7 +844,7 @@
         <v>3200</v>
       </c>
       <c r="D13" s="5">
-        <v>4800</v>
+        <v>2800</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -886,7 +853,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -906,7 +873,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="27" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
@@ -918,28 +885,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3:Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:17" ht="23.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -958,19 +925,19 @@
       <c r="F2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="17"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="Q2" s="11"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
         <v>6</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="8">
         <v>17.379054381320401</v>
       </c>
       <c r="E3" s="1">
@@ -980,17 +947,17 @@
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>2</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="8">
         <v>19.564456078774299</v>
       </c>
       <c r="E4" s="1">
@@ -1000,17 +967,17 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="8">
         <v>1</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>7</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="8">
         <v>1.9626754092080101</v>
       </c>
       <c r="E5" s="1">
@@ -1020,17 +987,17 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="8">
         <v>2</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>7</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="8">
         <v>16.612554040638301</v>
       </c>
       <c r="E6" s="1">
@@ -1040,17 +1007,17 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="8">
         <v>2</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>5</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="8">
         <v>6.0685871722204396</v>
       </c>
       <c r="E7" s="1">
@@ -1060,17 +1027,17 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="8">
         <v>3</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>5</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="8">
         <v>11.130284881867601</v>
       </c>
       <c r="E8" s="1">
@@ -1080,17 +1047,17 @@
         <v>600</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="8">
         <v>3</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="8">
         <v>4</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>6.3793126545787198</v>
       </c>
       <c r="E9" s="1">
@@ -1100,17 +1067,17 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="8">
         <v>4</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>5</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>25.275407155214999</v>
       </c>
       <c r="E10" s="1">
@@ -1120,17 +1087,17 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="8">
         <v>5</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <v>8</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <v>25.597686788240299</v>
       </c>
       <c r="E11" s="1">
@@ -1140,17 +1107,17 @@
         <v>2095</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="8">
         <v>6</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>7</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="8">
         <v>65.121040477936305</v>
       </c>
       <c r="E12" s="1">
@@ -1160,17 +1127,17 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="8">
         <v>6</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="8">
         <v>10</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="8">
         <v>32.080287978329103</v>
       </c>
       <c r="E13" s="1">
@@ -1180,17 +1147,17 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="8">
         <v>7</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="8">
         <v>8</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="8">
         <v>118.761657941248</v>
       </c>
       <c r="E14" s="1">
@@ -1200,17 +1167,17 @@
         <v>7300</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="8">
         <v>8</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="8">
         <v>9</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="8">
         <v>125.98550587149199</v>
       </c>
       <c r="E15" s="1">
@@ -1220,17 +1187,17 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="8">
         <v>9</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="8">
         <v>12</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="8">
         <v>63.909769630844401</v>
       </c>
       <c r="E16" s="1">
@@ -1240,105 +1207,77 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
         <v>15</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="8">
         <v>8</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="8">
         <v>11</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="10">
         <v>17.458315129999999</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="1">
         <v>680</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="1">
         <v>740</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="10"/>
-      <c r="D34" s="9"/>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1357,23 +1296,23 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="5" max="6" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="5" max="6" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:6" ht="23.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1387,7 +1326,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1401,31 +1340,31 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="8">
         <v>4</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>11</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="8">
         <v>1632</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="8">
         <v>11</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>12</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="8">
         <v>600</v>
       </c>
     </row>
@@ -1442,26 +1381,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="37.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
@@ -1475,21 +1414,21 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1503,7 +1442,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1517,7 +1456,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1525,7 +1464,7 @@
         <v>35</v>
       </c>
       <c r="C6">
-        <v>3000</v>
+        <v>3200</v>
       </c>
       <c r="D6" t="s">
         <v>39</v>

</xml_diff>